<commit_message>
lieu thu phi git 20k
</commit_message>
<xml_diff>
--- a/selenium_1/src/main/java/DataObjects/loginAccount.xlsx
+++ b/selenium_1/src/main/java/DataObjects/loginAccount.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
   <si>
     <t>Login</t>
   </si>
@@ -25,13 +26,34 @@
   </si>
   <si>
     <t>thanhle@logigear.com</t>
+  </si>
+  <si>
+    <t>Sài Gòn</t>
+  </si>
+  <si>
+    <t>Book Ticket</t>
+  </si>
+  <si>
+    <t>6/26/2021</t>
+  </si>
+  <si>
+    <t>Phan Thiết</t>
+  </si>
+  <si>
+    <t>Soft seat</t>
+  </si>
+  <si>
+    <t>Login fail</t>
+  </si>
+  <si>
+    <t>rerfh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -46,6 +68,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -69,9 +97,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -376,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,24 +465,198 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>25456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3">
+        <v>12345678</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>25456</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>